<commit_message>
Add more tests and plots
</commit_message>
<xml_diff>
--- a/SSQOL-results.xlsx
+++ b/SSQOL-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steff\Documents\GitHub\MED10_DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1759BA23-A4F1-40B1-A3D4-BBCE3BF40CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E4408-22B7-4324-8B34-CA9C4F7C4AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1742,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E803F574-52DE-459A-806B-73003564887F}">
   <dimension ref="A1:G358"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
+      <selection activeCell="J355" sqref="J355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4404,7 +4404,7 @@
         <v>3</v>
       </c>
       <c r="G129" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -4423,7 +4423,7 @@
       <c r="E130" s="6"/>
       <c r="F130" s="6"/>
       <c r="G130" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4442,7 +4442,7 @@
       <c r="E131" s="6"/>
       <c r="F131" s="6"/>
       <c r="G131" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
       <c r="E132" s="6"/>
       <c r="F132" s="6"/>
       <c r="G132" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4484,7 +4484,7 @@
         <v>3</v>
       </c>
       <c r="G133" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -4503,7 +4503,7 @@
       <c r="E134" s="6"/>
       <c r="F134" s="6"/>
       <c r="G134" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4526,7 +4526,7 @@
         <v>4</v>
       </c>
       <c r="G135" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -4545,7 +4545,7 @@
       <c r="E136" s="6"/>
       <c r="F136" s="6"/>
       <c r="G136" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4568,7 +4568,7 @@
         <v>3</v>
       </c>
       <c r="G137" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -4587,7 +4587,7 @@
       <c r="E138" s="6"/>
       <c r="F138" s="6"/>
       <c r="G138" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -4606,7 +4606,7 @@
       <c r="E139" s="6"/>
       <c r="F139" s="6"/>
       <c r="G139" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -4629,7 +4629,7 @@
         <v>2</v>
       </c>
       <c r="G140" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -4648,7 +4648,7 @@
       <c r="E141" s="6"/>
       <c r="F141" s="6"/>
       <c r="G141" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>5</v>
       </c>
       <c r="G142" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -4690,7 +4690,7 @@
       <c r="E143" s="6"/>
       <c r="F143" s="6"/>
       <c r="G143" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -4713,7 +4713,7 @@
         <v>5</v>
       </c>
       <c r="G144" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -4732,7 +4732,7 @@
       <c r="E145" s="6"/>
       <c r="F145" s="6"/>
       <c r="G145" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4755,7 +4755,7 @@
         <v>5</v>
       </c>
       <c r="G146" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -4774,7 +4774,7 @@
       <c r="E147" s="6"/>
       <c r="F147" s="6"/>
       <c r="G147" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -4797,7 +4797,7 @@
         <v>4</v>
       </c>
       <c r="G148" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -4816,7 +4816,7 @@
       <c r="E149" s="6"/>
       <c r="F149" s="6"/>
       <c r="G149" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -4835,7 +4835,7 @@
       <c r="E150" s="6"/>
       <c r="F150" s="6"/>
       <c r="G150" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -4858,7 +4858,7 @@
         <v>3</v>
       </c>
       <c r="G151" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -4877,7 +4877,7 @@
       <c r="E152" s="6"/>
       <c r="F152" s="6"/>
       <c r="G152" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -4900,7 +4900,7 @@
         <v>3</v>
       </c>
       <c r="G153" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -4919,7 +4919,7 @@
       <c r="E154" s="6"/>
       <c r="F154" s="6"/>
       <c r="G154" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -4942,7 +4942,7 @@
         <v>3</v>
       </c>
       <c r="G155" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -4961,7 +4961,7 @@
       <c r="E156" s="6"/>
       <c r="F156" s="6"/>
       <c r="G156" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4984,7 +4984,7 @@
         <v>3</v>
       </c>
       <c r="G157" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5003,7 +5003,7 @@
       <c r="E158" s="6"/>
       <c r="F158" s="6"/>
       <c r="G158" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -5026,7 +5026,7 @@
         <v>2</v>
       </c>
       <c r="G159" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5045,7 +5045,7 @@
       <c r="E160" s="6"/>
       <c r="F160" s="6"/>
       <c r="G160" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5064,7 +5064,7 @@
       <c r="E161" s="6"/>
       <c r="F161" s="6"/>
       <c r="G161" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -5087,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="G162" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
       <c r="E163" s="6"/>
       <c r="F163" s="6"/>
       <c r="G163" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5129,7 +5129,7 @@
         <v>2</v>
       </c>
       <c r="G164" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5148,7 +5148,7 @@
       <c r="E165" s="6"/>
       <c r="F165" s="6"/>
       <c r="G165" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -5171,7 +5171,7 @@
         <v>5</v>
       </c>
       <c r="G166" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5190,7 +5190,7 @@
       <c r="E167" s="6"/>
       <c r="F167" s="6"/>
       <c r="G167" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -5213,7 +5213,7 @@
         <v>3</v>
       </c>
       <c r="G168" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5232,7 +5232,7 @@
       <c r="E169" s="6"/>
       <c r="F169" s="6"/>
       <c r="G169" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -5255,7 +5255,7 @@
         <v>4</v>
       </c>
       <c r="G170" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5274,7 +5274,7 @@
       <c r="E171" s="6"/>
       <c r="F171" s="6"/>
       <c r="G171" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5293,7 +5293,7 @@
       <c r="E172" s="6"/>
       <c r="F172" s="6"/>
       <c r="G172" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -5316,7 +5316,7 @@
         <v>3</v>
       </c>
       <c r="G173" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5335,7 +5335,7 @@
       <c r="E174" s="6"/>
       <c r="F174" s="6"/>
       <c r="G174" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -5358,7 +5358,7 @@
         <v>3</v>
       </c>
       <c r="G175" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5377,7 +5377,7 @@
       <c r="E176" s="6"/>
       <c r="F176" s="6"/>
       <c r="G176" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -5400,7 +5400,7 @@
         <v>2</v>
       </c>
       <c r="G177" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5419,7 +5419,7 @@
       <c r="E178" s="6"/>
       <c r="F178" s="6"/>
       <c r="G178" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -5442,7 +5442,7 @@
         <v>2</v>
       </c>
       <c r="G179" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5461,7 +5461,7 @@
       <c r="E180" s="6"/>
       <c r="F180" s="6"/>
       <c r="G180" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5480,7 +5480,7 @@
       <c r="E181" s="6"/>
       <c r="F181" s="6"/>
       <c r="G181" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -5503,7 +5503,7 @@
         <v>1</v>
       </c>
       <c r="G182" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5522,7 +5522,7 @@
       <c r="E183" s="6"/>
       <c r="F183" s="6"/>
       <c r="G183" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -5541,7 +5541,7 @@
       <c r="E184" s="6"/>
       <c r="F184" s="6"/>
       <c r="G184" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
@@ -5560,7 +5560,7 @@
       <c r="E185" s="6"/>
       <c r="F185" s="6"/>
       <c r="G185" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -5583,7 +5583,7 @@
         <v>2</v>
       </c>
       <c r="G186" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5602,7 +5602,7 @@
       <c r="E187" s="6"/>
       <c r="F187" s="6"/>
       <c r="G187" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -5625,7 +5625,7 @@
         <v>3</v>
       </c>
       <c r="G188" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5644,7 +5644,7 @@
       <c r="E189" s="6"/>
       <c r="F189" s="6"/>
       <c r="G189" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -5667,7 +5667,7 @@
         <v>2</v>
       </c>
       <c r="G190" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5686,7 +5686,7 @@
       <c r="E191" s="6"/>
       <c r="F191" s="6"/>
       <c r="G191" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -5709,7 +5709,7 @@
         <v>2</v>
       </c>
       <c r="G192" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5728,7 +5728,7 @@
       <c r="E193" s="6"/>
       <c r="F193" s="6"/>
       <c r="G193" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -5751,7 +5751,7 @@
         <v>1</v>
       </c>
       <c r="G194" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="195" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5770,7 +5770,7 @@
       <c r="E195" s="6"/>
       <c r="F195" s="6"/>
       <c r="G195" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5789,7 +5789,7 @@
       <c r="E196" s="6"/>
       <c r="F196" s="6"/>
       <c r="G196" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -5812,7 +5812,7 @@
         <v>1</v>
       </c>
       <c r="G197" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5831,7 +5831,7 @@
       <c r="E198" s="6"/>
       <c r="F198" s="6"/>
       <c r="G198" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -5854,7 +5854,7 @@
         <v>1</v>
       </c>
       <c r="G199" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -5873,7 +5873,7 @@
       <c r="E200" s="6"/>
       <c r="F200" s="6"/>
       <c r="G200" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -5896,7 +5896,7 @@
         <v>1</v>
       </c>
       <c r="G201" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5915,7 +5915,7 @@
       <c r="E202" s="6"/>
       <c r="F202" s="6"/>
       <c r="G202" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -5934,7 +5934,7 @@
       <c r="E203" s="6"/>
       <c r="F203" s="6"/>
       <c r="G203" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -5953,7 +5953,7 @@
       <c r="E204" s="6"/>
       <c r="F204" s="6"/>
       <c r="G204" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -5976,7 +5976,7 @@
         <v>2</v>
       </c>
       <c r="G205" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="206" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -5995,7 +5995,7 @@
       <c r="E206" s="6"/>
       <c r="F206" s="6"/>
       <c r="G206" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -6018,7 +6018,7 @@
         <v>1</v>
       </c>
       <c r="G207" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="208" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6037,7 +6037,7 @@
       <c r="E208" s="6"/>
       <c r="F208" s="6"/>
       <c r="G208" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="209" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -6056,7 +6056,7 @@
       <c r="E209" s="6"/>
       <c r="F209" s="6"/>
       <c r="G209" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -6079,7 +6079,7 @@
         <v>4</v>
       </c>
       <c r="G210" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6098,7 +6098,7 @@
       <c r="E211" s="6"/>
       <c r="F211" s="6"/>
       <c r="G211" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6121,7 +6121,7 @@
         <v>1</v>
       </c>
       <c r="G212" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6140,7 +6140,7 @@
       <c r="E213" s="6"/>
       <c r="F213" s="6"/>
       <c r="G213" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -6163,7 +6163,7 @@
         <v>1</v>
       </c>
       <c r="G214" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="215" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -6182,7 +6182,7 @@
       <c r="E215" s="6"/>
       <c r="F215" s="6"/>
       <c r="G215" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6205,7 +6205,7 @@
         <v>1</v>
       </c>
       <c r="G216" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="217" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6224,7 +6224,7 @@
       <c r="E217" s="6"/>
       <c r="F217" s="6"/>
       <c r="G217" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -6247,7 +6247,7 @@
         <v>1</v>
       </c>
       <c r="G218" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6266,7 +6266,7 @@
       <c r="E219" s="6"/>
       <c r="F219" s="6"/>
       <c r="G219" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -6285,7 +6285,7 @@
       <c r="E220" s="6"/>
       <c r="F220" s="6"/>
       <c r="G220" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -6308,7 +6308,7 @@
         <v>1</v>
       </c>
       <c r="G221" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="222" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -6327,7 +6327,7 @@
       <c r="E222" s="6"/>
       <c r="F222" s="6"/>
       <c r="G222" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -6350,7 +6350,7 @@
         <v>5</v>
       </c>
       <c r="G223" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="224" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -6369,7 +6369,7 @@
       <c r="E224" s="6"/>
       <c r="F224" s="6"/>
       <c r="G224" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -6392,7 +6392,7 @@
         <v>1</v>
       </c>
       <c r="G225" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="226" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6411,7 +6411,7 @@
       <c r="E226" s="6"/>
       <c r="F226" s="6"/>
       <c r="G226" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -6434,7 +6434,7 @@
         <v>1</v>
       </c>
       <c r="G227" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="228" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6453,7 +6453,7 @@
       <c r="E228" s="6"/>
       <c r="F228" s="6"/>
       <c r="G228" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -6476,7 +6476,7 @@
         <v>4</v>
       </c>
       <c r="G229" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="230" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6495,7 +6495,7 @@
       <c r="E230" s="6"/>
       <c r="F230" s="6"/>
       <c r="G230" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="231" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6514,7 +6514,7 @@
       <c r="E231" s="6"/>
       <c r="F231" s="6"/>
       <c r="G231" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -6537,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="G232" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6556,7 +6556,7 @@
       <c r="E233" s="6"/>
       <c r="F233" s="6"/>
       <c r="G233" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -6579,7 +6579,7 @@
         <v>1</v>
       </c>
       <c r="G234" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="235" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -6598,7 +6598,7 @@
       <c r="E235" s="6"/>
       <c r="F235" s="6"/>
       <c r="G235" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -6621,7 +6621,7 @@
         <v>5</v>
       </c>
       <c r="G236" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="237" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6640,7 +6640,7 @@
       <c r="E237" s="6"/>
       <c r="F237" s="6"/>
       <c r="G237" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -6663,7 +6663,7 @@
         <v>1</v>
       </c>
       <c r="G238" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="239" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6682,7 +6682,7 @@
       <c r="E239" s="6"/>
       <c r="F239" s="6"/>
       <c r="G239" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="240" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -6701,7 +6701,7 @@
       <c r="E240" s="6"/>
       <c r="F240" s="6"/>
       <c r="G240" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -6724,7 +6724,7 @@
         <v>2</v>
       </c>
       <c r="G241" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="242" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -6743,7 +6743,7 @@
       <c r="E242" s="6"/>
       <c r="F242" s="6"/>
       <c r="G242" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="243" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -6762,7 +6762,7 @@
       <c r="E243" s="6"/>
       <c r="F243" s="6"/>
       <c r="G243" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -6785,7 +6785,7 @@
         <v>5</v>
       </c>
       <c r="G244" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="245" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -6802,7 +6802,7 @@
         <v>7</v>
       </c>
       <c r="G245" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -6825,7 +6825,7 @@
         <v>5</v>
       </c>
       <c r="G246" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="247" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -6842,7 +6842,7 @@
         <v>10</v>
       </c>
       <c r="G247" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -6865,7 +6865,7 @@
         <v>5</v>
       </c>
       <c r="G248" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="249" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -6882,7 +6882,7 @@
         <v>16</v>
       </c>
       <c r="G249" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -6905,7 +6905,7 @@
         <v>4</v>
       </c>
       <c r="G250" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="251" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -6922,7 +6922,7 @@
         <v>327</v>
       </c>
       <c r="G251" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="252" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -6939,7 +6939,7 @@
         <v>20</v>
       </c>
       <c r="G252" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -6962,7 +6962,7 @@
         <v>5</v>
       </c>
       <c r="G253" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="254" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -6979,7 +6979,7 @@
         <v>23</v>
       </c>
       <c r="G254" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -7002,7 +7002,7 @@
         <v>5</v>
       </c>
       <c r="G255" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="256" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7019,7 +7019,7 @@
         <v>26</v>
       </c>
       <c r="G256" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -7042,7 +7042,7 @@
         <v>4</v>
       </c>
       <c r="G257" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="258" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7059,7 +7059,7 @@
         <v>332</v>
       </c>
       <c r="G258" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
@@ -7082,7 +7082,7 @@
         <v>4</v>
       </c>
       <c r="G259" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="260" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7099,7 +7099,7 @@
         <v>335</v>
       </c>
       <c r="G260" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -7122,7 +7122,7 @@
         <v>4</v>
       </c>
       <c r="G261" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="262" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7139,7 +7139,7 @@
         <v>207</v>
       </c>
       <c r="G262" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="263" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7156,7 +7156,7 @@
         <v>36</v>
       </c>
       <c r="G263" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
@@ -7179,7 +7179,7 @@
         <v>5</v>
       </c>
       <c r="G264" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="265" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7196,7 +7196,7 @@
         <v>39</v>
       </c>
       <c r="G265" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
@@ -7213,7 +7213,7 @@
         <v>339</v>
       </c>
       <c r="G266" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="267" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7230,7 +7230,7 @@
         <v>340</v>
       </c>
       <c r="G267" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
@@ -7247,7 +7247,7 @@
         <v>339</v>
       </c>
       <c r="G268" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="269" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7264,7 +7264,7 @@
         <v>340</v>
       </c>
       <c r="G269" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
@@ -7287,7 +7287,7 @@
         <v>5</v>
       </c>
       <c r="G270" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="271" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7304,7 +7304,7 @@
         <v>42</v>
       </c>
       <c r="G271" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
@@ -7327,7 +7327,7 @@
         <v>4</v>
       </c>
       <c r="G272" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="273" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7344,7 +7344,7 @@
         <v>48</v>
       </c>
       <c r="G273" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
@@ -7367,7 +7367,7 @@
         <v>3</v>
       </c>
       <c r="G274" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="275" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7384,7 +7384,7 @@
         <v>219</v>
       </c>
       <c r="G275" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
@@ -7401,7 +7401,7 @@
         <v>346</v>
       </c>
       <c r="G276" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="277" spans="1:7" ht="77.25" x14ac:dyDescent="0.25">
@@ -7418,7 +7418,7 @@
         <v>84</v>
       </c>
       <c r="G277" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
@@ -7435,7 +7435,7 @@
         <v>348</v>
       </c>
       <c r="G278" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="279" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7452,7 +7452,7 @@
         <v>87</v>
       </c>
       <c r="G279" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="280" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7469,7 +7469,7 @@
         <v>88</v>
       </c>
       <c r="G280" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -7492,7 +7492,7 @@
         <v>3</v>
       </c>
       <c r="G281" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="282" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7509,7 +7509,7 @@
         <v>62</v>
       </c>
       <c r="G282" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
@@ -7532,7 +7532,7 @@
         <v>3</v>
       </c>
       <c r="G283" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="284" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7549,7 +7549,7 @@
         <v>65</v>
       </c>
       <c r="G284" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
@@ -7572,7 +7572,7 @@
         <v>4</v>
       </c>
       <c r="G285" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="286" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7589,7 +7589,7 @@
         <v>353</v>
       </c>
       <c r="G286" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
@@ -7612,7 +7612,7 @@
         <v>4</v>
       </c>
       <c r="G287" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="288" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7629,7 +7629,7 @@
         <v>71</v>
       </c>
       <c r="G288" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
@@ -7652,7 +7652,7 @@
         <v>4</v>
       </c>
       <c r="G289" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="290" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7669,7 +7669,7 @@
         <v>74</v>
       </c>
       <c r="G290" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="291" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7686,7 +7686,7 @@
         <v>75</v>
       </c>
       <c r="G291" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
@@ -7709,7 +7709,7 @@
         <v>3</v>
       </c>
       <c r="G292" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="293" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7726,7 +7726,7 @@
         <v>236</v>
       </c>
       <c r="G293" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
@@ -7749,7 +7749,7 @@
         <v>2</v>
       </c>
       <c r="G294" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="295" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7766,7 +7766,7 @@
         <v>359</v>
       </c>
       <c r="G295" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
@@ -7789,7 +7789,7 @@
         <v>4</v>
       </c>
       <c r="G296" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="297" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7806,7 +7806,7 @@
         <v>91</v>
       </c>
       <c r="G297" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
@@ -7829,7 +7829,7 @@
         <v>3</v>
       </c>
       <c r="G298" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="299" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7846,7 +7846,7 @@
         <v>363</v>
       </c>
       <c r="G299" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="300" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7863,7 +7863,7 @@
         <v>95</v>
       </c>
       <c r="G300" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.25">
@@ -7886,7 +7886,7 @@
         <v>2</v>
       </c>
       <c r="G301" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="302" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -7903,7 +7903,7 @@
         <v>366</v>
       </c>
       <c r="G302" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.25">
@@ -7926,7 +7926,7 @@
         <v>4</v>
       </c>
       <c r="G303" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="304" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7943,7 +7943,7 @@
         <v>101</v>
       </c>
       <c r="G304" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
@@ -7966,7 +7966,7 @@
         <v>5</v>
       </c>
       <c r="G305" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="306" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -7983,7 +7983,7 @@
         <v>370</v>
       </c>
       <c r="G306" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
@@ -8006,7 +8006,7 @@
         <v>5</v>
       </c>
       <c r="G307" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="308" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8023,7 +8023,7 @@
         <v>373</v>
       </c>
       <c r="G308" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
@@ -8046,7 +8046,7 @@
         <v>1</v>
       </c>
       <c r="G309" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="310" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8063,7 +8063,7 @@
         <v>262</v>
       </c>
       <c r="G310" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="311" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8080,7 +8080,7 @@
         <v>117</v>
       </c>
       <c r="G311" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
@@ -8103,7 +8103,7 @@
         <v>2</v>
       </c>
       <c r="G312" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="313" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8120,7 +8120,7 @@
         <v>111</v>
       </c>
       <c r="G313" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
@@ -8143,7 +8143,7 @@
         <v>1</v>
       </c>
       <c r="G314" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="315" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8160,7 +8160,7 @@
         <v>120</v>
       </c>
       <c r="G315" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.25">
@@ -8183,7 +8183,7 @@
         <v>5</v>
       </c>
       <c r="G316" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="317" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8200,7 +8200,7 @@
         <v>379</v>
       </c>
       <c r="G317" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
@@ -8223,7 +8223,7 @@
         <v>5</v>
       </c>
       <c r="G318" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="319" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8240,7 +8240,7 @@
         <v>382</v>
       </c>
       <c r="G319" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.25">
@@ -8263,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="G320" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="321" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8280,7 +8280,7 @@
         <v>129</v>
       </c>
       <c r="G321" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.25">
@@ -8303,7 +8303,7 @@
         <v>5</v>
       </c>
       <c r="G322" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="323" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8320,7 +8320,7 @@
         <v>386</v>
       </c>
       <c r="G323" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="324" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8337,7 +8337,7 @@
         <v>133</v>
       </c>
       <c r="G324" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.25">
@@ -8360,7 +8360,7 @@
         <v>4</v>
       </c>
       <c r="G325" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="326" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8377,7 +8377,7 @@
         <v>280</v>
       </c>
       <c r="G326" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.25">
@@ -8400,7 +8400,7 @@
         <v>2</v>
       </c>
       <c r="G327" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="328" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8417,7 +8417,7 @@
         <v>390</v>
       </c>
       <c r="G328" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.25">
@@ -8440,7 +8440,7 @@
         <v>3</v>
       </c>
       <c r="G329" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="330" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8457,7 +8457,7 @@
         <v>142</v>
       </c>
       <c r="G330" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.25">
@@ -8480,7 +8480,7 @@
         <v>4</v>
       </c>
       <c r="G331" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="332" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8497,7 +8497,7 @@
         <v>394</v>
       </c>
       <c r="G332" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.25">
@@ -8520,7 +8520,7 @@
         <v>2</v>
       </c>
       <c r="G333" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="334" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8537,7 +8537,7 @@
         <v>148</v>
       </c>
       <c r="G334" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="335" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8554,7 +8554,7 @@
         <v>149</v>
       </c>
       <c r="G335" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.25">
@@ -8577,7 +8577,7 @@
         <v>1</v>
       </c>
       <c r="G336" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="337" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8594,7 +8594,7 @@
         <v>152</v>
       </c>
       <c r="G337" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.25">
@@ -8617,7 +8617,7 @@
         <v>5</v>
       </c>
       <c r="G338" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="339" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8634,7 +8634,7 @@
         <v>297</v>
       </c>
       <c r="G339" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.25">
@@ -8657,7 +8657,7 @@
         <v>5</v>
       </c>
       <c r="G340" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="341" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8674,7 +8674,7 @@
         <v>400</v>
       </c>
       <c r="G341" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.25">
@@ -8697,7 +8697,7 @@
         <v>4</v>
       </c>
       <c r="G342" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="343" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8714,7 +8714,7 @@
         <v>403</v>
       </c>
       <c r="G343" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.25">
@@ -8737,7 +8737,7 @@
         <v>4</v>
       </c>
       <c r="G344" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="345" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8754,7 +8754,7 @@
         <v>306</v>
       </c>
       <c r="G345" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="346" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8771,7 +8771,7 @@
         <v>167</v>
       </c>
       <c r="G346" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.25">
@@ -8794,7 +8794,7 @@
         <v>4</v>
       </c>
       <c r="G347" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="348" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8811,7 +8811,7 @@
         <v>407</v>
       </c>
       <c r="G348" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -8834,7 +8834,7 @@
         <v>2</v>
       </c>
       <c r="G349" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="350" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8851,7 +8851,7 @@
         <v>410</v>
       </c>
       <c r="G350" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
@@ -8874,7 +8874,7 @@
         <v>5</v>
       </c>
       <c r="G351" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="352" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8891,7 +8891,7 @@
         <v>413</v>
       </c>
       <c r="G352" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
@@ -8914,7 +8914,7 @@
         <v>1</v>
       </c>
       <c r="G353" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="354" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -8931,7 +8931,7 @@
         <v>317</v>
       </c>
       <c r="G354" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="355" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8948,7 +8948,7 @@
         <v>180</v>
       </c>
       <c r="G355" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.25">
@@ -8971,7 +8971,7 @@
         <v>1</v>
       </c>
       <c r="G356" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="357" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -8988,7 +8988,7 @@
         <v>417</v>
       </c>
       <c r="G357" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="358" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
@@ -9005,7 +9005,7 @@
         <v>184</v>
       </c>
       <c r="G358" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>